<commit_message>
feat: add texas demo
</commit_message>
<xml_diff>
--- a/gameconf/xlsx/router.xlsx
+++ b/gameconf/xlsx/router.xlsx
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="97">
   <si>
     <t>Cmd</t>
   </si>
@@ -179,6 +179,132 @@
   </si>
   <si>
     <t>心跳请求</t>
+  </si>
+  <si>
+    <t>0x3000000</t>
+  </si>
+  <si>
+    <t>节点类型-Match</t>
+  </si>
+  <si>
+    <t>路由类型-GameType</t>
+  </si>
+  <si>
+    <t>TexasRoomListReq</t>
+  </si>
+  <si>
+    <t>TexasRoomListRsp</t>
+  </si>
+  <si>
+    <t>TexasRoom</t>
+  </si>
+  <si>
+    <t>RoomListReq</t>
+  </si>
+  <si>
+    <t>德州房间列表请求</t>
+  </si>
+  <si>
+    <t>0x4000000</t>
+  </si>
+  <si>
+    <t>节点类型-Room</t>
+  </si>
+  <si>
+    <t>路由类型-RoomId</t>
+  </si>
+  <si>
+    <t>TexasEventNotify</t>
+  </si>
+  <si>
+    <t>德州扑克游戏通知请求</t>
+  </si>
+  <si>
+    <t>0x4000002</t>
+  </si>
+  <si>
+    <t>TexasJoinRoomReq</t>
+  </si>
+  <si>
+    <t>TexasJoinRoomRsp</t>
+  </si>
+  <si>
+    <t>PlayerMgr</t>
+  </si>
+  <si>
+    <t>德州扑克加入房间请求</t>
+  </si>
+  <si>
+    <t>0x4000004</t>
+  </si>
+  <si>
+    <t>TexasQuitRoomReq</t>
+  </si>
+  <si>
+    <t>TexasQuitRoomRsp</t>
+  </si>
+  <si>
+    <t>离开房间</t>
+  </si>
+  <si>
+    <t>0x4000006</t>
+  </si>
+  <si>
+    <t>TexasSitDownReq</t>
+  </si>
+  <si>
+    <t>TexasSitDownRsp</t>
+  </si>
+  <si>
+    <t>TexasGameMgr</t>
+  </si>
+  <si>
+    <t>SitDownReq</t>
+  </si>
+  <si>
+    <t>坐下请求</t>
+  </si>
+  <si>
+    <t>0x4000008</t>
+  </si>
+  <si>
+    <t>TexasStandUpReq</t>
+  </si>
+  <si>
+    <t>TexasStandUpRsp</t>
+  </si>
+  <si>
+    <t>StandUpReq</t>
+  </si>
+  <si>
+    <t>站起请求</t>
+  </si>
+  <si>
+    <t>0x4000010</t>
+  </si>
+  <si>
+    <t>TexasBuyInReq</t>
+  </si>
+  <si>
+    <t>TexasBuyInRsp</t>
+  </si>
+  <si>
+    <t>买入请求</t>
+  </si>
+  <si>
+    <t>0x4000012</t>
+  </si>
+  <si>
+    <t>TexasDoBetReq</t>
+  </si>
+  <si>
+    <t>TexasDoBetRsp</t>
+  </si>
+  <si>
+    <t>DoBetReq</t>
+  </si>
+  <si>
+    <t>下注请求</t>
   </si>
   <si>
     <t>E|节点类型-begin|NodeType|Begin|0</t>
@@ -433,7 +559,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,6 +569,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -780,7 +924,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -804,16 +948,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -822,89 +966,89 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -915,6 +1059,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1235,13 +1388,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="21.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
@@ -1376,6 +1529,208 @@
       </c>
       <c r="H5" s="3" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1403,70 +1758,70 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1492,42 +1847,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>